<commit_message>
- map & + progress bar
</commit_message>
<xml_diff>
--- a/nadda_progress.xlsx
+++ b/nadda_progress.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTILITY RELOCATION\extra\web app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Office\2. NKB\Utility\web app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F2C3A6-5C0A-4BDF-AFEC-582713B2846F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D0E92A-0D89-49BC-973C-74F4B2BC7607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Corridor Work" sheetId="2" r:id="rId1"/>
     <sheet name="Progress" sheetId="4" r:id="rId2"/>
     <sheet name="Remaining" sheetId="1" r:id="rId3"/>
     <sheet name="Issue Log" sheetId="3" r:id="rId4"/>
+    <sheet name="images" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="61">
   <si>
     <t>Corridor</t>
   </si>
@@ -178,6 +190,39 @@
   </si>
   <si>
     <t>400mm</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>update_date</t>
+  </si>
+  <si>
+    <t>s05/plan.jpg</t>
+  </si>
+  <si>
+    <t>s05/HA1-HA1'.jpg</t>
+  </si>
+  <si>
+    <t>s05/HA2-HA2'.jpg</t>
+  </si>
+  <si>
+    <t>s05/HA3-HA3'.jpg</t>
+  </si>
+  <si>
+    <t>s05/HA4-HA4'.jpg</t>
+  </si>
+  <si>
+    <t>s05/C12-C12'.jpg</t>
+  </si>
+  <si>
+    <t>s05/C13-C13'.jpg</t>
+  </si>
+  <si>
+    <t>s05/C13A-C13A'.jpg</t>
+  </si>
+  <si>
+    <t>s05/C13B-C13B'.jpg</t>
   </si>
 </sst>
 </file>
@@ -542,16 +587,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341F8D72-1DB1-4E58-BF84-59E9EEAD3E98}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2367,7 +2412,7 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -4428,10 +4473,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4503,14 +4548,14 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4637,4 +4682,105 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF461C2-E285-45A5-9187-EE76ED3492E9}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45757</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>